<commit_message>
Lightmaps Baked on L1&L2, L1 Canvas changed
</commit_message>
<xml_diff>
--- a/User Testing/Responses.xlsx
+++ b/User Testing/Responses.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\3000\Timeline-Takedown\User Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E90741D-E536-4EAB-8343-0F7539BFCADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6041D88-CC71-4DEE-993D-622DDE617CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="555" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Test1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,9 +25,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test 1 : </t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Did you understand the games mechanics quickly?</t>
+  </si>
+  <si>
+    <t>Responses</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Were there any unclear or confusing mechanics</t>
+  </si>
+  <si>
+    <t>How did you find the levels difficulty</t>
+  </si>
+  <si>
+    <t>How Buggy did the game feel</t>
+  </si>
+  <si>
+    <t>Not that I'm aware of</t>
+  </si>
+  <si>
+    <t>Very easy, most enemies died in one hit</t>
+  </si>
+  <si>
+    <t>Not at all</t>
+  </si>
+  <si>
+    <t>Boss didn’t spawn</t>
+  </si>
+  <si>
+    <t>How would you rate the visual design of the game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Did the levels enviroment feel enaging and emmersive </t>
+  </si>
+  <si>
+    <t>Were there any graphical or audio issues? If so, please describe them.</t>
+  </si>
+  <si>
+    <t>7/10 strong theme</t>
+  </si>
+  <si>
+    <t>I liked the buildings that you could go in and explore. The terrain looked really cool as well.</t>
+  </si>
+  <si>
+    <t>I liked exploring the pyramids, so yes</t>
+  </si>
+  <si>
+    <t>No reload animation</t>
+  </si>
+  <si>
+    <t>I saw some random flying objects</t>
+  </si>
+  <si>
+    <t>Did you enjoy playing this level?</t>
+  </si>
+  <si>
+    <t>Did you feel motivated to keep playing after completing the level?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> What improvements would you suggest for this level?</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>I'd be interested in seeing other levels, so yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maybe have a few more buildings to go inside of and explore. </t>
+  </si>
+  <si>
+    <t>The pyramids didn't have anything I could pick up, maybe add something in them that I can engage with</t>
+  </si>
+  <si>
+    <t>Testing Type: Excel Sheet</t>
   </si>
 </sst>
 </file>
@@ -51,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -59,12 +143,85 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,20 +502,131 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4"/>
+  <dimension ref="B3:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="3" customWidth="1"/>
+    <col min="4" max="4" width="3.5703125" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" customWidth="1"/>
+    <col min="7" max="7" width="36" customWidth="1"/>
+    <col min="8" max="8" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="8" t="s">
         <v>0</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="E14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="E15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="E16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>